<commit_message>
some changes and final
</commit_message>
<xml_diff>
--- a/pokemon_data.xlsx
+++ b/pokemon_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmetizmirlioglu/Library/Mobile Documents/com~apple~CloudDocs/Eğitim&amp;Öğretim/BAU21:22(1)/SEN4018 - Data Science with Python/jupyter-notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehmetizmirlioglu/Library/Mobile Documents/com~apple~CloudDocs/Eğitim&amp;Öğretim/BAU21:22(1)/SEN4018 - Data Science with Python/jupyter-notebook/pokemon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCD8871-FE3D-1640-A99B-F2D704F5B7B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410FE14A-9366-7949-A918-735716BFBE18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="1560" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1560" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pokemon_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="830">
   <si>
     <t>#</t>
   </si>
@@ -2515,6 +2515,9 @@
   </si>
   <si>
     <t>Hoopa Unbound</t>
+  </si>
+  <si>
+    <t>Primeape</t>
   </si>
 </sst>
 </file>
@@ -3331,8 +3334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L801"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:B801"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5649,7 +5652,9 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>829</v>
+      </c>
       <c r="C64" t="s">
         <v>77</v>
       </c>

</xml_diff>